<commit_message>
added 3030 print files
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM Beta 06.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM Beta 06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_B1EE2D6939D15B17C21F420868F9B71A58448DE0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{273232A1-0CF6-41B5-B6ED-9BF973ACD46D}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_B1EE2D6939D15B17C21F420868F9B71A58448DE0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B1C6E18-9AEF-4F9C-B2CF-B78384ABC9D8}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="314">
   <si>
     <t>PROJECT VALKYRIE</t>
   </si>
@@ -1520,6 +1520,12 @@
   </si>
   <si>
     <t>Cup Washer for Outer Panels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VenstPow </t>
+  </si>
+  <si>
+    <t>PIR - Polyisocyanurate</t>
   </si>
 </sst>
 </file>
@@ -2034,9 +2040,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2055,6 +2058,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2600,24 +2606,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="1"/>
@@ -2664,7 +2670,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="63">
         <f>J112</f>
-        <v>1839.4599999999998</v>
+        <v>1789.4599999999998</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="10"/>
@@ -3168,7 +3174,7 @@
         <v>41</v>
       </c>
       <c r="L19" s="83" t="s">
-        <v>28</v>
+        <v>312</v>
       </c>
       <c r="M19" s="84"/>
       <c r="N19" s="85"/>
@@ -4409,25 +4415,25 @@
       <c r="O49" s="54"/>
       <c r="P49" s="35"/>
     </row>
-    <row r="50" spans="1:16" s="90" customFormat="1">
-      <c r="A50" s="88" t="s">
+    <row r="50" spans="1:16" s="89" customFormat="1">
+      <c r="A50" s="87" t="s">
         <v>207</v>
       </c>
-      <c r="B50" s="89" t="s">
+      <c r="B50" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="89" t="s">
+      <c r="C50" s="88" t="s">
         <v>96</v>
       </c>
-      <c r="D50" s="90" t="s">
+      <c r="D50" s="89" t="s">
         <v>311</v>
       </c>
-      <c r="F50" s="91"/>
-      <c r="G50" s="91"/>
-      <c r="H50" s="92">
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="91">
         <v>8</v>
       </c>
-      <c r="I50" s="91">
+      <c r="I50" s="90">
         <v>1</v>
       </c>
       <c r="J50" s="31">
@@ -4437,51 +4443,51 @@
       <c r="K50" s="36" t="s">
         <v>310</v>
       </c>
-      <c r="L50" s="94" t="s">
+      <c r="L50" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="M50" s="95"/>
-      <c r="N50" s="95"/>
-      <c r="O50" s="96"/>
-      <c r="P50" s="97"/>
-    </row>
-    <row r="51" spans="1:16" s="90" customFormat="1">
-      <c r="A51" s="88" t="s">
+      <c r="M50" s="94"/>
+      <c r="N50" s="94"/>
+      <c r="O50" s="95"/>
+      <c r="P50" s="96"/>
+    </row>
+    <row r="51" spans="1:16" s="89" customFormat="1">
+      <c r="A51" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="B51" s="89" t="s">
+      <c r="B51" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="90" t="s">
+      <c r="C51" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="90" t="s">
+      <c r="D51" s="89" t="s">
         <v>307</v>
       </c>
-      <c r="F51" s="91"/>
-      <c r="G51" s="91"/>
-      <c r="H51" s="92">
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="91">
         <v>0.74</v>
       </c>
-      <c r="I51" s="91">
+      <c r="I51" s="90">
         <v>1</v>
       </c>
       <c r="J51" s="31">
         <f t="shared" si="1"/>
         <v>0.74</v>
       </c>
-      <c r="K51" s="93" t="s">
+      <c r="K51" s="92" t="s">
         <v>309</v>
       </c>
-      <c r="L51" s="94" t="s">
+      <c r="L51" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="M51" s="98" t="s">
+      <c r="M51" s="97" t="s">
         <v>308</v>
       </c>
-      <c r="N51" s="95"/>
-      <c r="O51" s="96"/>
-      <c r="P51" s="97"/>
+      <c r="N51" s="94"/>
+      <c r="O51" s="95"/>
+      <c r="P51" s="96"/>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="26" t="s">
@@ -5557,7 +5563,7 @@
         <v>208</v>
       </c>
       <c r="D79" s="38" t="s">
-        <v>200</v>
+        <v>313</v>
       </c>
       <c r="E79" s="27"/>
       <c r="F79" s="30"/>
@@ -5565,14 +5571,14 @@
         <v>5</v>
       </c>
       <c r="H79" s="31">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I79" s="39">
         <v>5</v>
       </c>
       <c r="J79" s="31">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="K79" s="36" t="s">
         <v>200</v>
@@ -5604,14 +5610,14 @@
         <v>5</v>
       </c>
       <c r="H80" s="31">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I80" s="39">
         <v>5</v>
       </c>
       <c r="J80" s="31">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="K80" s="36" t="s">
         <v>200</v>
@@ -6907,7 +6913,7 @@
       <c r="I112" s="18"/>
       <c r="J112" s="64">
         <f>SUM(J19:J111)</f>
-        <v>1839.4599999999998</v>
+        <v>1789.4599999999998</v>
       </c>
       <c r="K112" s="17"/>
       <c r="L112" s="19"/>

</xml_diff>